<commit_message>
add new stage for education
</commit_message>
<xml_diff>
--- a/sample_df.xlsx
+++ b/sample_df.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamerlan\Desktop\QSS Projects\TalentScoringBackend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C809D9EE-BCD6-42A0-96C9-9F1A2C6FE1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -805,8 +811,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -869,13 +875,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -913,7 +927,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -947,6 +961,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -981,9 +996,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1156,14 +1172,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1976</v>
       </c>
@@ -1275,7 +1293,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -1331,7 +1349,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -1387,7 +1405,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1976</v>
       </c>
@@ -1443,7 +1461,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2000</v>
       </c>
@@ -1499,7 +1517,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1993</v>
       </c>
@@ -1555,7 +1573,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1996</v>
       </c>
@@ -1611,7 +1629,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1985</v>
       </c>
@@ -1667,7 +1685,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2014</v>
       </c>
@@ -1723,7 +1741,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1991</v>
       </c>
@@ -1779,7 +1797,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -1835,7 +1853,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -1891,7 +1909,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1990</v>
       </c>
@@ -1947,7 +1965,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -2003,7 +2021,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1989</v>
       </c>
@@ -2059,7 +2077,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2009</v>
       </c>
@@ -2115,7 +2133,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2012</v>
       </c>
@@ -2171,7 +2189,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1974</v>
       </c>
@@ -2227,7 +2245,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1989</v>
       </c>
@@ -2283,7 +2301,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2009</v>
       </c>
@@ -2339,7 +2357,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2012</v>
       </c>
@@ -2395,7 +2413,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1996</v>
       </c>
@@ -2451,7 +2469,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2007</v>
       </c>
@@ -2507,7 +2525,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2009</v>
       </c>
@@ -2563,7 +2581,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1992</v>
       </c>
@@ -2619,7 +2637,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1974</v>
       </c>
@@ -2675,7 +2693,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1999</v>
       </c>
@@ -2731,7 +2749,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2002</v>
       </c>
@@ -2787,7 +2805,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1985</v>
       </c>
@@ -2843,7 +2861,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1986</v>
       </c>
@@ -2899,7 +2917,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1980</v>
       </c>
@@ -2955,7 +2973,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1983</v>
       </c>
@@ -3011,7 +3029,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1989</v>
       </c>
@@ -3067,7 +3085,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1983</v>
       </c>
@@ -3123,7 +3141,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -3179,7 +3197,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2008</v>
       </c>
@@ -3235,7 +3253,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1986</v>
       </c>
@@ -3291,7 +3309,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1992</v>
       </c>
@@ -3347,7 +3365,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2000</v>
       </c>
@@ -3403,7 +3421,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1992</v>
       </c>
@@ -3459,7 +3477,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1990</v>
       </c>
@@ -3515,7 +3533,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2013</v>
       </c>
@@ -3571,7 +3589,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2003</v>
       </c>
@@ -3627,7 +3645,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1987</v>
       </c>
@@ -3683,7 +3701,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -3739,7 +3757,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2009</v>
       </c>
@@ -3795,7 +3813,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1998</v>
       </c>
@@ -3851,7 +3869,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1984</v>
       </c>
@@ -3907,7 +3925,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1977</v>
       </c>
@@ -3963,7 +3981,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1994</v>
       </c>

</xml_diff>